<commit_message>
added scroll action for methods in family cover
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UltimateDignityPlan.xlsx
+++ b/src/test/resources/TestData/UltimateDignityPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="78">
   <si>
     <t>IDNumber</t>
   </si>
@@ -137,6 +137,117 @@
   </si>
   <si>
     <t>0105053304082</t>
+  </si>
+  <si>
+    <t>9505052351086</t>
+  </si>
+  <si>
+    <t>9105050675188</t>
+  </si>
+  <si>
+    <t>0105050484184</t>
+  </si>
+  <si>
+    <t>9805054281087</t>
+  </si>
+  <si>
+    <t>9505053023189</t>
+  </si>
+  <si>
+    <t>0105052534085</t>
+  </si>
+  <si>
+    <t>9805050350183</t>
+  </si>
+  <si>
+    <t>9505053406186</t>
+  </si>
+  <si>
+    <t>0105054378085</t>
+  </si>
+  <si>
+    <t>9805052525188</t>
+  </si>
+  <si>
+    <t>9505052006185</t>
+  </si>
+  <si>
+    <t>0105050624185</t>
+  </si>
+  <si>
+    <t>9805051782186</t>
+  </si>
+  <si>
+    <t>9505051784089</t>
+  </si>
+  <si>
+    <t>0105051766084</t>
+  </si>
+  <si>
+    <t>9805054945186</t>
+  </si>
+  <si>
+    <t>9505050169183</t>
+  </si>
+  <si>
+    <t>0105050261186</t>
+  </si>
+  <si>
+    <t>9805051382185</t>
+  </si>
+  <si>
+    <t>9505052228086</t>
+  </si>
+  <si>
+    <t>9105051715181</t>
+  </si>
+  <si>
+    <t>0105051775085</t>
+  </si>
+  <si>
+    <t>98050509840810</t>
+  </si>
+  <si>
+    <t>9505050884187</t>
+  </si>
+  <si>
+    <t>0105051542089</t>
+  </si>
+  <si>
+    <t>9805051204082</t>
+  </si>
+  <si>
+    <t>9505052650081</t>
+  </si>
+  <si>
+    <t>0105054410185</t>
+  </si>
+  <si>
+    <t>9805052254086</t>
+  </si>
+  <si>
+    <t>9505053769088</t>
+  </si>
+  <si>
+    <t>0105050666186</t>
+  </si>
+  <si>
+    <t>9805050541088</t>
+  </si>
+  <si>
+    <t>9505053958087</t>
+  </si>
+  <si>
+    <t>0105050939088</t>
+  </si>
+  <si>
+    <t>9805050872186</t>
+  </si>
+  <si>
+    <t>9505052887188</t>
+  </si>
+  <si>
+    <t>0105052266084</t>
   </si>
 </sst>
 </file>
@@ -487,7 +598,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -823,6 +934,302 @@
         <v>4</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="s" s="1">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="1">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="1">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="1">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="1">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="1">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="1">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="1">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="1">
+        <v>50</v>
+      </c>
+      <c r="C50" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="1">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="1">
+        <v>52</v>
+      </c>
+      <c r="C52" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="1">
+        <v>53</v>
+      </c>
+      <c r="C53" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="1">
+        <v>54</v>
+      </c>
+      <c r="C54" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="1">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="1">
+        <v>56</v>
+      </c>
+      <c r="C56" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="1">
+        <v>57</v>
+      </c>
+      <c r="C57" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="1">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="1">
+        <v>59</v>
+      </c>
+      <c r="C59" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
+        <v>60</v>
+      </c>
+      <c r="C60" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="1">
+        <v>61</v>
+      </c>
+      <c r="C61" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="1">
+        <v>62</v>
+      </c>
+      <c r="C62" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="C63" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="C64" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="C65" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="C66" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="1">
+        <v>67</v>
+      </c>
+      <c r="C67" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="1">
+        <v>68</v>
+      </c>
+      <c r="C68" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="1">
+        <v>69</v>
+      </c>
+      <c r="C69" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="C70" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="1">
+        <v>71</v>
+      </c>
+      <c r="C71" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="C72" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="1">
+        <v>73</v>
+      </c>
+      <c r="C73" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="1">
+        <v>74</v>
+      </c>
+      <c r="C74" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="1">
+        <v>75</v>
+      </c>
+      <c r="C75" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="1">
+        <v>76</v>
+      </c>
+      <c r="C76" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="1">
+        <v>77</v>
+      </c>
+      <c r="C77" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated project framework version
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UltimateDignityPlan.xlsx
+++ b/src/test/resources/TestData/UltimateDignityPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82075" uniqueCount="414">
   <si>
     <t>IDNumber</t>
   </si>
@@ -248,6 +248,1014 @@
   </si>
   <si>
     <t>0105052266084</t>
+  </si>
+  <si>
+    <t>0105053279185</t>
+  </si>
+  <si>
+    <t>98050517991810</t>
+  </si>
+  <si>
+    <t>9505053104187</t>
+  </si>
+  <si>
+    <t>0105050197083</t>
+  </si>
+  <si>
+    <t>9805050505083</t>
+  </si>
+  <si>
+    <t>9505053461181</t>
+  </si>
+  <si>
+    <t>9105051648184</t>
+  </si>
+  <si>
+    <t>9405054171089</t>
+  </si>
+  <si>
+    <t>9005053129185</t>
+  </si>
+  <si>
+    <t>8705053036089</t>
+  </si>
+  <si>
+    <t>8505052378189</t>
+  </si>
+  <si>
+    <t>8405053506187</t>
+  </si>
+  <si>
+    <t>8305054173187</t>
+  </si>
+  <si>
+    <t>8205052518187</t>
+  </si>
+  <si>
+    <t>8005054530085</t>
+  </si>
+  <si>
+    <t>7905053102086</t>
+  </si>
+  <si>
+    <t>7805053414186</t>
+  </si>
+  <si>
+    <t>7705051931084</t>
+  </si>
+  <si>
+    <t>7605050927085</t>
+  </si>
+  <si>
+    <t>7505054042081</t>
+  </si>
+  <si>
+    <t>7405051361081</t>
+  </si>
+  <si>
+    <t>7305054989088</t>
+  </si>
+  <si>
+    <t>7205052132188</t>
+  </si>
+  <si>
+    <t>7105052751088</t>
+  </si>
+  <si>
+    <t>7005052099183</t>
+  </si>
+  <si>
+    <t>6905051063182</t>
+  </si>
+  <si>
+    <t>6805053409187</t>
+  </si>
+  <si>
+    <t>67050522590810</t>
+  </si>
+  <si>
+    <t>6605050429083</t>
+  </si>
+  <si>
+    <t>6505051782086</t>
+  </si>
+  <si>
+    <t>6405052010183</t>
+  </si>
+  <si>
+    <t>63050509190810</t>
+  </si>
+  <si>
+    <t>6205050060085</t>
+  </si>
+  <si>
+    <t>0105053992183</t>
+  </si>
+  <si>
+    <t>9805050033185</t>
+  </si>
+  <si>
+    <t>9505050156081</t>
+  </si>
+  <si>
+    <t>9405054292182</t>
+  </si>
+  <si>
+    <t>9005053647186</t>
+  </si>
+  <si>
+    <t>8705051648182</t>
+  </si>
+  <si>
+    <t>85050534001810</t>
+  </si>
+  <si>
+    <t>8405053545086</t>
+  </si>
+  <si>
+    <t>8305053758087</t>
+  </si>
+  <si>
+    <t>8205054701187</t>
+  </si>
+  <si>
+    <t>8005050594085</t>
+  </si>
+  <si>
+    <t>7905050244188</t>
+  </si>
+  <si>
+    <t>7805050979082</t>
+  </si>
+  <si>
+    <t>7705054221186</t>
+  </si>
+  <si>
+    <t>7605054606081</t>
+  </si>
+  <si>
+    <t>7505051834183</t>
+  </si>
+  <si>
+    <t>7405052286089</t>
+  </si>
+  <si>
+    <t>7305053012189</t>
+  </si>
+  <si>
+    <t>7205053235089</t>
+  </si>
+  <si>
+    <t>7105051877181</t>
+  </si>
+  <si>
+    <t>7005051820183</t>
+  </si>
+  <si>
+    <t>6905051131187</t>
+  </si>
+  <si>
+    <t>68050530351810</t>
+  </si>
+  <si>
+    <t>6705050065083</t>
+  </si>
+  <si>
+    <t>6605052267085</t>
+  </si>
+  <si>
+    <t>6505051241083</t>
+  </si>
+  <si>
+    <t>6405051037187</t>
+  </si>
+  <si>
+    <t>6305050298089</t>
+  </si>
+  <si>
+    <t>6205050516086</t>
+  </si>
+  <si>
+    <t>0105051736087</t>
+  </si>
+  <si>
+    <t>9805054563088</t>
+  </si>
+  <si>
+    <t>9505050011088</t>
+  </si>
+  <si>
+    <t>9305053721183</t>
+  </si>
+  <si>
+    <t>9005050168087</t>
+  </si>
+  <si>
+    <t>8705051682181</t>
+  </si>
+  <si>
+    <t>8405053368182</t>
+  </si>
+  <si>
+    <t>8305052507089</t>
+  </si>
+  <si>
+    <t>8205054761082</t>
+  </si>
+  <si>
+    <t>8005052635183</t>
+  </si>
+  <si>
+    <t>7905054827087</t>
+  </si>
+  <si>
+    <t>7805052209181</t>
+  </si>
+  <si>
+    <t>77050517961810</t>
+  </si>
+  <si>
+    <t>7605054315188</t>
+  </si>
+  <si>
+    <t>7505054057188</t>
+  </si>
+  <si>
+    <t>7405054301084</t>
+  </si>
+  <si>
+    <t>7305051686083</t>
+  </si>
+  <si>
+    <t>72050514480810</t>
+  </si>
+  <si>
+    <t>7105051133189</t>
+  </si>
+  <si>
+    <t>7005054703188</t>
+  </si>
+  <si>
+    <t>6905052538083</t>
+  </si>
+  <si>
+    <t>6805051001085</t>
+  </si>
+  <si>
+    <t>6705050743085</t>
+  </si>
+  <si>
+    <t>6605052568185</t>
+  </si>
+  <si>
+    <t>6505053615185</t>
+  </si>
+  <si>
+    <t>6405052827081</t>
+  </si>
+  <si>
+    <t>6305053387186</t>
+  </si>
+  <si>
+    <t>6205054322085</t>
+  </si>
+  <si>
+    <t>0105054421083</t>
+  </si>
+  <si>
+    <t>9805051386087</t>
+  </si>
+  <si>
+    <t>9505053828181</t>
+  </si>
+  <si>
+    <t>9305053046086</t>
+  </si>
+  <si>
+    <t>9005050792183</t>
+  </si>
+  <si>
+    <t>8705054688086</t>
+  </si>
+  <si>
+    <t>8505052806189</t>
+  </si>
+  <si>
+    <t>8405051245085</t>
+  </si>
+  <si>
+    <t>83050543221810</t>
+  </si>
+  <si>
+    <t>8205053106081</t>
+  </si>
+  <si>
+    <t>80050500060810</t>
+  </si>
+  <si>
+    <t>7905052351189</t>
+  </si>
+  <si>
+    <t>7805054035089</t>
+  </si>
+  <si>
+    <t>7705051767082</t>
+  </si>
+  <si>
+    <t>7605053657184</t>
+  </si>
+  <si>
+    <t>0105051718184</t>
+  </si>
+  <si>
+    <t>0105054367088</t>
+  </si>
+  <si>
+    <t>9805053503085</t>
+  </si>
+  <si>
+    <t>9505054675185</t>
+  </si>
+  <si>
+    <t>9405053148187</t>
+  </si>
+  <si>
+    <t>9005050773183</t>
+  </si>
+  <si>
+    <t>8705052414188</t>
+  </si>
+  <si>
+    <t>8505052757184</t>
+  </si>
+  <si>
+    <t>0105053146087</t>
+  </si>
+  <si>
+    <t>9805053851088</t>
+  </si>
+  <si>
+    <t>0105053075088</t>
+  </si>
+  <si>
+    <t>9805052990085</t>
+  </si>
+  <si>
+    <t>9505052635181</t>
+  </si>
+  <si>
+    <t>9405052279181</t>
+  </si>
+  <si>
+    <t>9505050204188</t>
+  </si>
+  <si>
+    <t>9005050507086</t>
+  </si>
+  <si>
+    <t>9405052267087</t>
+  </si>
+  <si>
+    <t>8705051816086</t>
+  </si>
+  <si>
+    <t>90050501281810</t>
+  </si>
+  <si>
+    <t>8505053748083</t>
+  </si>
+  <si>
+    <t>8705052612187</t>
+  </si>
+  <si>
+    <t>8505050181189</t>
+  </si>
+  <si>
+    <t>8405051362088</t>
+  </si>
+  <si>
+    <t>8405052135087</t>
+  </si>
+  <si>
+    <t>8305054975185</t>
+  </si>
+  <si>
+    <t>8305051602188</t>
+  </si>
+  <si>
+    <t>8205054878183</t>
+  </si>
+  <si>
+    <t>8205050360186</t>
+  </si>
+  <si>
+    <t>8005051505189</t>
+  </si>
+  <si>
+    <t>8005050826081</t>
+  </si>
+  <si>
+    <t>7905054638187</t>
+  </si>
+  <si>
+    <t>7905053658087</t>
+  </si>
+  <si>
+    <t>7805052847188</t>
+  </si>
+  <si>
+    <t>7805050414189</t>
+  </si>
+  <si>
+    <t>7705052570188</t>
+  </si>
+  <si>
+    <t>7705054801086</t>
+  </si>
+  <si>
+    <t>7605050231082</t>
+  </si>
+  <si>
+    <t>7605051983186</t>
+  </si>
+  <si>
+    <t>7505051630185</t>
+  </si>
+  <si>
+    <t>7505052727089</t>
+  </si>
+  <si>
+    <t>7405053206185</t>
+  </si>
+  <si>
+    <t>7405052522186</t>
+  </si>
+  <si>
+    <t>73050522341810</t>
+  </si>
+  <si>
+    <t>7205053311088</t>
+  </si>
+  <si>
+    <t>7305051380083</t>
+  </si>
+  <si>
+    <t>7205050292182</t>
+  </si>
+  <si>
+    <t>7105050364082</t>
+  </si>
+  <si>
+    <t>7005051844183</t>
+  </si>
+  <si>
+    <t>7105051523181</t>
+  </si>
+  <si>
+    <t>7005051832089</t>
+  </si>
+  <si>
+    <t>6905051755183</t>
+  </si>
+  <si>
+    <t>6905050481187</t>
+  </si>
+  <si>
+    <t>6805054614082</t>
+  </si>
+  <si>
+    <t>6805050610183</t>
+  </si>
+  <si>
+    <t>6705053947188</t>
+  </si>
+  <si>
+    <t>6705053897086</t>
+  </si>
+  <si>
+    <t>6605054274188</t>
+  </si>
+  <si>
+    <t>6605052106184</t>
+  </si>
+  <si>
+    <t>6505050584186</t>
+  </si>
+  <si>
+    <t>6505052530088</t>
+  </si>
+  <si>
+    <t>6405050696181</t>
+  </si>
+  <si>
+    <t>6405054793083</t>
+  </si>
+  <si>
+    <t>6305053404189</t>
+  </si>
+  <si>
+    <t>6305053834187</t>
+  </si>
+  <si>
+    <t>6205052209185</t>
+  </si>
+  <si>
+    <t>6205054197081</t>
+  </si>
+  <si>
+    <t>01050547950810</t>
+  </si>
+  <si>
+    <t>0105051933189</t>
+  </si>
+  <si>
+    <t>9805051966185</t>
+  </si>
+  <si>
+    <t>9805050073181</t>
+  </si>
+  <si>
+    <t>9505052877189</t>
+  </si>
+  <si>
+    <t>9405052591189</t>
+  </si>
+  <si>
+    <t>9405054105186</t>
+  </si>
+  <si>
+    <t>9005050150085</t>
+  </si>
+  <si>
+    <t>9005054335088</t>
+  </si>
+  <si>
+    <t>8705052277189</t>
+  </si>
+  <si>
+    <t>8705054708082</t>
+  </si>
+  <si>
+    <t>8505054486188</t>
+  </si>
+  <si>
+    <t>8405052002089</t>
+  </si>
+  <si>
+    <t>8405051789082</t>
+  </si>
+  <si>
+    <t>8305050934186</t>
+  </si>
+  <si>
+    <t>8305053005182</t>
+  </si>
+  <si>
+    <t>8205051158183</t>
+  </si>
+  <si>
+    <t>8205051447081</t>
+  </si>
+  <si>
+    <t>80050500680810</t>
+  </si>
+  <si>
+    <t>8005053985181</t>
+  </si>
+  <si>
+    <t>7905053573088</t>
+  </si>
+  <si>
+    <t>7905050665085</t>
+  </si>
+  <si>
+    <t>7805054445189</t>
+  </si>
+  <si>
+    <t>7805052953184</t>
+  </si>
+  <si>
+    <t>7705052506083</t>
+  </si>
+  <si>
+    <t>76050549891810</t>
+  </si>
+  <si>
+    <t>7505051781087</t>
+  </si>
+  <si>
+    <t>0105052163182</t>
+  </si>
+  <si>
+    <t>7405052350182</t>
+  </si>
+  <si>
+    <t>7305053857088</t>
+  </si>
+  <si>
+    <t>7205052188081</t>
+  </si>
+  <si>
+    <t>7105054287081</t>
+  </si>
+  <si>
+    <t>7005053838084</t>
+  </si>
+  <si>
+    <t>6905051066086</t>
+  </si>
+  <si>
+    <t>6805054338187</t>
+  </si>
+  <si>
+    <t>6705050189081</t>
+  </si>
+  <si>
+    <t>0105051771084</t>
+  </si>
+  <si>
+    <t>6605050089184</t>
+  </si>
+  <si>
+    <t>6505054838083</t>
+  </si>
+  <si>
+    <t>6405053381088</t>
+  </si>
+  <si>
+    <t>6305052415186</t>
+  </si>
+  <si>
+    <t>62050535510810</t>
+  </si>
+  <si>
+    <t>0105050335188</t>
+  </si>
+  <si>
+    <t>9805052872085</t>
+  </si>
+  <si>
+    <t>0105051504089</t>
+  </si>
+  <si>
+    <t>9505051079084</t>
+  </si>
+  <si>
+    <t>9105053239081</t>
+  </si>
+  <si>
+    <t>9405051026088</t>
+  </si>
+  <si>
+    <t>9005050846088</t>
+  </si>
+  <si>
+    <t>01050513101810</t>
+  </si>
+  <si>
+    <t>8705053746182</t>
+  </si>
+  <si>
+    <t>8505050785088</t>
+  </si>
+  <si>
+    <t>8405052793083</t>
+  </si>
+  <si>
+    <t>8305054522086</t>
+  </si>
+  <si>
+    <t>8205051658083</t>
+  </si>
+  <si>
+    <t>0105054985186</t>
+  </si>
+  <si>
+    <t>9805052804187</t>
+  </si>
+  <si>
+    <t>8005054875183</t>
+  </si>
+  <si>
+    <t>7905050939084</t>
+  </si>
+  <si>
+    <t>78050535730810</t>
+  </si>
+  <si>
+    <t>7705052177182</t>
+  </si>
+  <si>
+    <t>0105054420085</t>
+  </si>
+  <si>
+    <t>9805054976181</t>
+  </si>
+  <si>
+    <t>7505053987088</t>
+  </si>
+  <si>
+    <t>7405054501188</t>
+  </si>
+  <si>
+    <t>7305053234189</t>
+  </si>
+  <si>
+    <t>7205051678181</t>
+  </si>
+  <si>
+    <t>7105050282086</t>
+  </si>
+  <si>
+    <t>6805052587082</t>
+  </si>
+  <si>
+    <t>6705050784188</t>
+  </si>
+  <si>
+    <t>6605050122084</t>
+  </si>
+  <si>
+    <t>6505050985185</t>
+  </si>
+  <si>
+    <t>6405051254188</t>
+  </si>
+  <si>
+    <t>63050522011810</t>
+  </si>
+  <si>
+    <t>6205051497187</t>
+  </si>
+  <si>
+    <t>0105053634082</t>
+  </si>
+  <si>
+    <t>9805054960086</t>
+  </si>
+  <si>
+    <t>9505053911086</t>
+  </si>
+  <si>
+    <t>9405053654184</t>
+  </si>
+  <si>
+    <t>9005050893189</t>
+  </si>
+  <si>
+    <t>87050530641810</t>
+  </si>
+  <si>
+    <t>8505054124185</t>
+  </si>
+  <si>
+    <t>8405050152084</t>
+  </si>
+  <si>
+    <t>83050532000810</t>
+  </si>
+  <si>
+    <t>8205053263189</t>
+  </si>
+  <si>
+    <t>80050545420810</t>
+  </si>
+  <si>
+    <t>7905053135086</t>
+  </si>
+  <si>
+    <t>7805050013189</t>
+  </si>
+  <si>
+    <t>7705053753189</t>
+  </si>
+  <si>
+    <t>7605053106182</t>
+  </si>
+  <si>
+    <t>7505050391086</t>
+  </si>
+  <si>
+    <t>0105051130083</t>
+  </si>
+  <si>
+    <t>74050506540810</t>
+  </si>
+  <si>
+    <t>0105053380181</t>
+  </si>
+  <si>
+    <t>7305054082082</t>
+  </si>
+  <si>
+    <t>7205050497088</t>
+  </si>
+  <si>
+    <t>7105053449187</t>
+  </si>
+  <si>
+    <t>7005054145083</t>
+  </si>
+  <si>
+    <t>6905051412082</t>
+  </si>
+  <si>
+    <t>6805053868184</t>
+  </si>
+  <si>
+    <t>6705050346186</t>
+  </si>
+  <si>
+    <t>6605050677087</t>
+  </si>
+  <si>
+    <t>6505051760181</t>
+  </si>
+  <si>
+    <t>64050511210810</t>
+  </si>
+  <si>
+    <t>6305050215182</t>
+  </si>
+  <si>
+    <t>6205053327085</t>
+  </si>
+  <si>
+    <t>0105052500086</t>
+  </si>
+  <si>
+    <t>9805050724189</t>
+  </si>
+  <si>
+    <t>9505053738182</t>
+  </si>
+  <si>
+    <t>9305052727181</t>
+  </si>
+  <si>
+    <t>9005054481189</t>
+  </si>
+  <si>
+    <t>8705050189089</t>
+  </si>
+  <si>
+    <t>8505050549187</t>
+  </si>
+  <si>
+    <t>84050514451810</t>
+  </si>
+  <si>
+    <t>8305054527184</t>
+  </si>
+  <si>
+    <t>8205050651089</t>
+  </si>
+  <si>
+    <t>8005050226084</t>
+  </si>
+  <si>
+    <t>7905050079089</t>
+  </si>
+  <si>
+    <t>7805053263187</t>
+  </si>
+  <si>
+    <t>7705054260085</t>
+  </si>
+  <si>
+    <t>76050525461810</t>
+  </si>
+  <si>
+    <t>7505054675187</t>
+  </si>
+  <si>
+    <t>74050514080810</t>
+  </si>
+  <si>
+    <t>7305050950183</t>
+  </si>
+  <si>
+    <t>7205050154085</t>
+  </si>
+  <si>
+    <t>7105051195188</t>
+  </si>
+  <si>
+    <t>7005053218089</t>
+  </si>
+  <si>
+    <t>6905050562085</t>
+  </si>
+  <si>
+    <t>6805051832182</t>
+  </si>
+  <si>
+    <t>6705051974085</t>
+  </si>
+  <si>
+    <t>6605053255188</t>
+  </si>
+  <si>
+    <t>6505050063082</t>
+  </si>
+  <si>
+    <t>6405053736182</t>
+  </si>
+  <si>
+    <t>6305054923088</t>
+  </si>
+  <si>
+    <t>6205051827185</t>
+  </si>
+  <si>
+    <t>01050548560810</t>
+  </si>
+  <si>
+    <t>9805050943185</t>
+  </si>
+  <si>
+    <t>9505050043081</t>
+  </si>
+  <si>
+    <t>93050505500810</t>
+  </si>
+  <si>
+    <t>9005052267085</t>
+  </si>
+  <si>
+    <t>8705051733182</t>
+  </si>
+  <si>
+    <t>85050539661810</t>
+  </si>
+  <si>
+    <t>8405052546085</t>
+  </si>
+  <si>
+    <t>8305050862189</t>
+  </si>
+  <si>
+    <t>8205051415187</t>
+  </si>
+  <si>
+    <t>8005050286187</t>
+  </si>
+  <si>
+    <t>7905051143082</t>
+  </si>
+  <si>
+    <t>7805050321087</t>
+  </si>
+  <si>
+    <t>7705051753181</t>
+  </si>
+  <si>
+    <t>7605052633087</t>
+  </si>
+  <si>
+    <t>75050549240810</t>
+  </si>
+  <si>
+    <t>7405052888082</t>
+  </si>
+  <si>
+    <t>7305051535082</t>
+  </si>
+  <si>
+    <t>7205053983183</t>
+  </si>
+  <si>
+    <t>7105053736088</t>
+  </si>
+  <si>
+    <t>7005052296086</t>
+  </si>
+  <si>
+    <t>6905053637082</t>
+  </si>
+  <si>
+    <t>6805050604186</t>
+  </si>
+  <si>
+    <t>6705054321185</t>
+  </si>
+  <si>
+    <t>6605054468186</t>
+  </si>
+  <si>
+    <t>6505050485186</t>
+  </si>
+  <si>
+    <t>6405051587181</t>
+  </si>
+  <si>
+    <t>6305050393088</t>
+  </si>
+  <si>
+    <t>62050540981810</t>
+  </si>
+  <si>
+    <t>0105052090187</t>
   </si>
 </sst>
 </file>
@@ -598,7 +1606,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C413"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -1230,6 +2238,2691 @@
         <v>4</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="s" s="1">
+        <v>78</v>
+      </c>
+      <c r="C78" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="1">
+        <v>79</v>
+      </c>
+      <c r="C79" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="1">
+        <v>80</v>
+      </c>
+      <c r="C80" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="C81" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="1">
+        <v>82</v>
+      </c>
+      <c r="C82" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="1">
+        <v>83</v>
+      </c>
+      <c r="C83" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="1">
+        <v>84</v>
+      </c>
+      <c r="C84" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="1">
+        <v>85</v>
+      </c>
+      <c r="C85" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="1">
+        <v>86</v>
+      </c>
+      <c r="C86" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="1">
+        <v>87</v>
+      </c>
+      <c r="C87" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="C88" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="1">
+        <v>89</v>
+      </c>
+      <c r="C89" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="1">
+        <v>90</v>
+      </c>
+      <c r="C90" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="1">
+        <v>91</v>
+      </c>
+      <c r="C91" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="1">
+        <v>92</v>
+      </c>
+      <c r="C92" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="1">
+        <v>93</v>
+      </c>
+      <c r="C93" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="1">
+        <v>94</v>
+      </c>
+      <c r="C94" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="1">
+        <v>95</v>
+      </c>
+      <c r="C95" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="C96" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="1">
+        <v>97</v>
+      </c>
+      <c r="C97" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="1">
+        <v>98</v>
+      </c>
+      <c r="C98" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="1">
+        <v>99</v>
+      </c>
+      <c r="C99" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="1">
+        <v>100</v>
+      </c>
+      <c r="C100" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="1">
+        <v>101</v>
+      </c>
+      <c r="C101" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="1">
+        <v>102</v>
+      </c>
+      <c r="C102" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="1">
+        <v>103</v>
+      </c>
+      <c r="C103" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="1">
+        <v>104</v>
+      </c>
+      <c r="C104" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="1">
+        <v>105</v>
+      </c>
+      <c r="C105" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="1">
+        <v>106</v>
+      </c>
+      <c r="C106" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="1">
+        <v>107</v>
+      </c>
+      <c r="C107" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="1">
+        <v>108</v>
+      </c>
+      <c r="C108" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="1">
+        <v>109</v>
+      </c>
+      <c r="C109" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="1">
+        <v>110</v>
+      </c>
+      <c r="C110" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="1">
+        <v>111</v>
+      </c>
+      <c r="C111" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="1">
+        <v>112</v>
+      </c>
+      <c r="C112" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="1">
+        <v>113</v>
+      </c>
+      <c r="C113" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="1">
+        <v>114</v>
+      </c>
+      <c r="C114" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="1">
+        <v>115</v>
+      </c>
+      <c r="C115" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="1">
+        <v>116</v>
+      </c>
+      <c r="C116" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="1">
+        <v>117</v>
+      </c>
+      <c r="C117" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="1">
+        <v>118</v>
+      </c>
+      <c r="C118" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="1">
+        <v>119</v>
+      </c>
+      <c r="C119" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="1">
+        <v>120</v>
+      </c>
+      <c r="C120" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="1">
+        <v>121</v>
+      </c>
+      <c r="C121" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="1">
+        <v>122</v>
+      </c>
+      <c r="C122" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="1">
+        <v>123</v>
+      </c>
+      <c r="C123" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="1">
+        <v>124</v>
+      </c>
+      <c r="C124" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="1">
+        <v>125</v>
+      </c>
+      <c r="C125" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="1">
+        <v>126</v>
+      </c>
+      <c r="C126" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="1">
+        <v>127</v>
+      </c>
+      <c r="C127" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="1">
+        <v>128</v>
+      </c>
+      <c r="C128" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="1">
+        <v>129</v>
+      </c>
+      <c r="C129" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="1">
+        <v>130</v>
+      </c>
+      <c r="C130" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="1">
+        <v>131</v>
+      </c>
+      <c r="C131" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="1">
+        <v>132</v>
+      </c>
+      <c r="C132" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="1">
+        <v>133</v>
+      </c>
+      <c r="C133" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="1">
+        <v>134</v>
+      </c>
+      <c r="C134" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="1">
+        <v>135</v>
+      </c>
+      <c r="C135" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="1">
+        <v>136</v>
+      </c>
+      <c r="C136" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="1">
+        <v>137</v>
+      </c>
+      <c r="C137" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="1">
+        <v>138</v>
+      </c>
+      <c r="C138" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="1">
+        <v>139</v>
+      </c>
+      <c r="C139" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="1">
+        <v>140</v>
+      </c>
+      <c r="C140" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="1">
+        <v>141</v>
+      </c>
+      <c r="C141" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="1">
+        <v>142</v>
+      </c>
+      <c r="C142" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="1">
+        <v>143</v>
+      </c>
+      <c r="C143" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="1">
+        <v>144</v>
+      </c>
+      <c r="C144" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="1">
+        <v>145</v>
+      </c>
+      <c r="C145" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="1">
+        <v>146</v>
+      </c>
+      <c r="C146" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="1">
+        <v>147</v>
+      </c>
+      <c r="C147" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="1">
+        <v>148</v>
+      </c>
+      <c r="C148" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="1">
+        <v>149</v>
+      </c>
+      <c r="C149" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="1">
+        <v>150</v>
+      </c>
+      <c r="C150" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="1">
+        <v>151</v>
+      </c>
+      <c r="C151" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="1">
+        <v>152</v>
+      </c>
+      <c r="C152" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="1">
+        <v>153</v>
+      </c>
+      <c r="C153" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="1">
+        <v>154</v>
+      </c>
+      <c r="C154" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="1">
+        <v>155</v>
+      </c>
+      <c r="C155" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="1">
+        <v>156</v>
+      </c>
+      <c r="C156" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="1">
+        <v>157</v>
+      </c>
+      <c r="C157" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="1">
+        <v>158</v>
+      </c>
+      <c r="C158" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="1">
+        <v>159</v>
+      </c>
+      <c r="C159" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="1">
+        <v>160</v>
+      </c>
+      <c r="C160" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s" s="1">
+        <v>161</v>
+      </c>
+      <c r="C161" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="1">
+        <v>162</v>
+      </c>
+      <c r="C162" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="1">
+        <v>163</v>
+      </c>
+      <c r="C163" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s" s="1">
+        <v>164</v>
+      </c>
+      <c r="C164" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s" s="1">
+        <v>165</v>
+      </c>
+      <c r="C165" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="1">
+        <v>166</v>
+      </c>
+      <c r="C166" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s" s="1">
+        <v>167</v>
+      </c>
+      <c r="C167" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s" s="1">
+        <v>168</v>
+      </c>
+      <c r="C168" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s" s="1">
+        <v>169</v>
+      </c>
+      <c r="C169" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s" s="1">
+        <v>170</v>
+      </c>
+      <c r="C170" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s" s="1">
+        <v>171</v>
+      </c>
+      <c r="C171" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s" s="1">
+        <v>172</v>
+      </c>
+      <c r="C172" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s" s="1">
+        <v>173</v>
+      </c>
+      <c r="C173" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s" s="1">
+        <v>174</v>
+      </c>
+      <c r="C174" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s" s="1">
+        <v>175</v>
+      </c>
+      <c r="C175" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s" s="1">
+        <v>176</v>
+      </c>
+      <c r="C176" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s" s="1">
+        <v>177</v>
+      </c>
+      <c r="C177" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s" s="1">
+        <v>178</v>
+      </c>
+      <c r="C178" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="C179" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s" s="1">
+        <v>180</v>
+      </c>
+      <c r="C180" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s" s="1">
+        <v>181</v>
+      </c>
+      <c r="C181" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="C182" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s" s="1">
+        <v>183</v>
+      </c>
+      <c r="C183" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s" s="1">
+        <v>184</v>
+      </c>
+      <c r="C184" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s" s="1">
+        <v>185</v>
+      </c>
+      <c r="C185" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s" s="1">
+        <v>186</v>
+      </c>
+      <c r="C186" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s" s="1">
+        <v>187</v>
+      </c>
+      <c r="C187" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s" s="1">
+        <v>188</v>
+      </c>
+      <c r="C188" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s" s="1">
+        <v>189</v>
+      </c>
+      <c r="C189" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="C190" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s" s="1">
+        <v>191</v>
+      </c>
+      <c r="C191" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s" s="1">
+        <v>192</v>
+      </c>
+      <c r="C192" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s" s="1">
+        <v>193</v>
+      </c>
+      <c r="C193" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s" s="1">
+        <v>194</v>
+      </c>
+      <c r="C194" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s" s="1">
+        <v>195</v>
+      </c>
+      <c r="C195" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s" s="1">
+        <v>196</v>
+      </c>
+      <c r="C196" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s" s="1">
+        <v>197</v>
+      </c>
+      <c r="C197" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s" s="1">
+        <v>198</v>
+      </c>
+      <c r="C198" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s" s="1">
+        <v>199</v>
+      </c>
+      <c r="C199" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s" s="1">
+        <v>200</v>
+      </c>
+      <c r="C200" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s" s="1">
+        <v>201</v>
+      </c>
+      <c r="C201" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s" s="1">
+        <v>202</v>
+      </c>
+      <c r="C202" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s" s="1">
+        <v>203</v>
+      </c>
+      <c r="C203" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s" s="1">
+        <v>204</v>
+      </c>
+      <c r="C204" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s" s="1">
+        <v>205</v>
+      </c>
+      <c r="C205" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s" s="1">
+        <v>206</v>
+      </c>
+      <c r="C206" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s" s="1">
+        <v>207</v>
+      </c>
+      <c r="C207" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s" s="1">
+        <v>208</v>
+      </c>
+      <c r="C208" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s" s="1">
+        <v>209</v>
+      </c>
+      <c r="C209" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s" s="1">
+        <v>210</v>
+      </c>
+      <c r="C210" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s" s="1">
+        <v>211</v>
+      </c>
+      <c r="C211" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s" s="1">
+        <v>212</v>
+      </c>
+      <c r="C212" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s" s="1">
+        <v>213</v>
+      </c>
+      <c r="C213" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s" s="1">
+        <v>214</v>
+      </c>
+      <c r="C214" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s" s="1">
+        <v>215</v>
+      </c>
+      <c r="C215" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s" s="1">
+        <v>216</v>
+      </c>
+      <c r="C216" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s" s="1">
+        <v>217</v>
+      </c>
+      <c r="C217" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s" s="1">
+        <v>218</v>
+      </c>
+      <c r="C218" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s" s="1">
+        <v>219</v>
+      </c>
+      <c r="C219" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s" s="1">
+        <v>220</v>
+      </c>
+      <c r="C220" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s" s="1">
+        <v>221</v>
+      </c>
+      <c r="C221" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s" s="1">
+        <v>222</v>
+      </c>
+      <c r="C222" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s" s="1">
+        <v>223</v>
+      </c>
+      <c r="C223" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s" s="1">
+        <v>224</v>
+      </c>
+      <c r="C224" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s" s="1">
+        <v>225</v>
+      </c>
+      <c r="C225" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s" s="1">
+        <v>226</v>
+      </c>
+      <c r="C226" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s" s="1">
+        <v>227</v>
+      </c>
+      <c r="C227" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s" s="1">
+        <v>228</v>
+      </c>
+      <c r="C228" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s" s="1">
+        <v>229</v>
+      </c>
+      <c r="C229" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s" s="1">
+        <v>230</v>
+      </c>
+      <c r="C230" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s" s="1">
+        <v>231</v>
+      </c>
+      <c r="C231" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s" s="1">
+        <v>232</v>
+      </c>
+      <c r="C232" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s" s="1">
+        <v>233</v>
+      </c>
+      <c r="C233" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s" s="1">
+        <v>234</v>
+      </c>
+      <c r="C234" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s" s="1">
+        <v>235</v>
+      </c>
+      <c r="C235" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s" s="1">
+        <v>236</v>
+      </c>
+      <c r="C236" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s" s="1">
+        <v>237</v>
+      </c>
+      <c r="C237" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s" s="1">
+        <v>238</v>
+      </c>
+      <c r="C238" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s" s="1">
+        <v>239</v>
+      </c>
+      <c r="C239" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s" s="1">
+        <v>240</v>
+      </c>
+      <c r="C240" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s" s="1">
+        <v>241</v>
+      </c>
+      <c r="C241" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s" s="1">
+        <v>242</v>
+      </c>
+      <c r="C242" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s" s="1">
+        <v>243</v>
+      </c>
+      <c r="C243" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s" s="1">
+        <v>244</v>
+      </c>
+      <c r="C244" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s" s="1">
+        <v>245</v>
+      </c>
+      <c r="C245" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s" s="1">
+        <v>246</v>
+      </c>
+      <c r="C246" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s" s="1">
+        <v>247</v>
+      </c>
+      <c r="C247" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s" s="1">
+        <v>248</v>
+      </c>
+      <c r="C248" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s" s="1">
+        <v>249</v>
+      </c>
+      <c r="C249" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s" s="1">
+        <v>250</v>
+      </c>
+      <c r="C250" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s" s="1">
+        <v>251</v>
+      </c>
+      <c r="C251" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="C252" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="C253" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="C254" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="C255" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="C256" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="C257" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C258" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s" s="1">
+        <v>259</v>
+      </c>
+      <c r="C259" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C260" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s" s="1">
+        <v>261</v>
+      </c>
+      <c r="C261" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C262" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C263" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C264" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C265" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C266" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C267" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s" s="1">
+        <v>268</v>
+      </c>
+      <c r="C268" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C269" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C270" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s" s="1">
+        <v>271</v>
+      </c>
+      <c r="C271" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s" s="1">
+        <v>272</v>
+      </c>
+      <c r="C272" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s" s="1">
+        <v>273</v>
+      </c>
+      <c r="C273" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s" s="1">
+        <v>274</v>
+      </c>
+      <c r="C274" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s" s="1">
+        <v>275</v>
+      </c>
+      <c r="C275" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s" s="1">
+        <v>276</v>
+      </c>
+      <c r="C276" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s" s="1">
+        <v>277</v>
+      </c>
+      <c r="C277" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s" s="1">
+        <v>278</v>
+      </c>
+      <c r="C278" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s" s="1">
+        <v>279</v>
+      </c>
+      <c r="C279" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s" s="1">
+        <v>280</v>
+      </c>
+      <c r="C280" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s" s="1">
+        <v>281</v>
+      </c>
+      <c r="C281" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s" s="1">
+        <v>282</v>
+      </c>
+      <c r="C282" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s" s="1">
+        <v>283</v>
+      </c>
+      <c r="C283" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s" s="1">
+        <v>284</v>
+      </c>
+      <c r="C284" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s" s="1">
+        <v>285</v>
+      </c>
+      <c r="C285" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s" s="1">
+        <v>286</v>
+      </c>
+      <c r="C286" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s" s="1">
+        <v>287</v>
+      </c>
+      <c r="C287" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s" s="1">
+        <v>288</v>
+      </c>
+      <c r="C288" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s" s="1">
+        <v>289</v>
+      </c>
+      <c r="C289" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s" s="1">
+        <v>290</v>
+      </c>
+      <c r="C290" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s" s="1">
+        <v>291</v>
+      </c>
+      <c r="C291" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s" s="1">
+        <v>292</v>
+      </c>
+      <c r="C292" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s" s="1">
+        <v>293</v>
+      </c>
+      <c r="C293" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s" s="1">
+        <v>294</v>
+      </c>
+      <c r="C294" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s" s="1">
+        <v>295</v>
+      </c>
+      <c r="C295" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s" s="1">
+        <v>296</v>
+      </c>
+      <c r="C296" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s" s="1">
+        <v>297</v>
+      </c>
+      <c r="C297" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s" s="1">
+        <v>298</v>
+      </c>
+      <c r="C298" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s" s="1">
+        <v>299</v>
+      </c>
+      <c r="C299" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s" s="1">
+        <v>300</v>
+      </c>
+      <c r="C300" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s" s="1">
+        <v>301</v>
+      </c>
+      <c r="C301" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s" s="1">
+        <v>302</v>
+      </c>
+      <c r="C302" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s" s="1">
+        <v>303</v>
+      </c>
+      <c r="C303" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s" s="1">
+        <v>304</v>
+      </c>
+      <c r="C304" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s" s="1">
+        <v>305</v>
+      </c>
+      <c r="C305" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s" s="1">
+        <v>306</v>
+      </c>
+      <c r="C306" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s" s="1">
+        <v>307</v>
+      </c>
+      <c r="C307" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s" s="1">
+        <v>308</v>
+      </c>
+      <c r="C308" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s" s="1">
+        <v>309</v>
+      </c>
+      <c r="C309" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s" s="1">
+        <v>310</v>
+      </c>
+      <c r="C310" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s" s="1">
+        <v>311</v>
+      </c>
+      <c r="C311" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s" s="1">
+        <v>312</v>
+      </c>
+      <c r="C312" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s" s="1">
+        <v>313</v>
+      </c>
+      <c r="C313" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s" s="1">
+        <v>314</v>
+      </c>
+      <c r="C314" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s" s="1">
+        <v>315</v>
+      </c>
+      <c r="C315" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s" s="1">
+        <v>316</v>
+      </c>
+      <c r="C316" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s" s="1">
+        <v>317</v>
+      </c>
+      <c r="C317" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s" s="1">
+        <v>318</v>
+      </c>
+      <c r="C318" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s" s="1">
+        <v>319</v>
+      </c>
+      <c r="C319" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s" s="1">
+        <v>320</v>
+      </c>
+      <c r="C320" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s" s="1">
+        <v>321</v>
+      </c>
+      <c r="C321" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s" s="1">
+        <v>322</v>
+      </c>
+      <c r="C322" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s" s="1">
+        <v>323</v>
+      </c>
+      <c r="C323" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s" s="1">
+        <v>324</v>
+      </c>
+      <c r="C324" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s" s="1">
+        <v>325</v>
+      </c>
+      <c r="C325" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s" s="1">
+        <v>326</v>
+      </c>
+      <c r="C326" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s" s="1">
+        <v>327</v>
+      </c>
+      <c r="C327" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s" s="1">
+        <v>328</v>
+      </c>
+      <c r="C328" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s" s="1">
+        <v>329</v>
+      </c>
+      <c r="C329" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s" s="1">
+        <v>330</v>
+      </c>
+      <c r="C330" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s" s="1">
+        <v>331</v>
+      </c>
+      <c r="C331" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s" s="1">
+        <v>332</v>
+      </c>
+      <c r="C332" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s" s="1">
+        <v>333</v>
+      </c>
+      <c r="C333" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s" s="1">
+        <v>334</v>
+      </c>
+      <c r="C334" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s" s="1">
+        <v>335</v>
+      </c>
+      <c r="C335" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s" s="1">
+        <v>336</v>
+      </c>
+      <c r="C336" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s" s="1">
+        <v>337</v>
+      </c>
+      <c r="C337" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s" s="1">
+        <v>338</v>
+      </c>
+      <c r="C338" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s" s="1">
+        <v>339</v>
+      </c>
+      <c r="C339" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s" s="1">
+        <v>340</v>
+      </c>
+      <c r="C340" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s" s="1">
+        <v>341</v>
+      </c>
+      <c r="C341" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s" s="1">
+        <v>342</v>
+      </c>
+      <c r="C342" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s" s="1">
+        <v>343</v>
+      </c>
+      <c r="C343" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s" s="1">
+        <v>344</v>
+      </c>
+      <c r="C344" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s" s="1">
+        <v>345</v>
+      </c>
+      <c r="C345" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s" s="1">
+        <v>346</v>
+      </c>
+      <c r="C346" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s" s="1">
+        <v>347</v>
+      </c>
+      <c r="C347" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s" s="1">
+        <v>348</v>
+      </c>
+      <c r="C348" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s" s="1">
+        <v>349</v>
+      </c>
+      <c r="C349" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s" s="1">
+        <v>350</v>
+      </c>
+      <c r="C350" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s" s="1">
+        <v>351</v>
+      </c>
+      <c r="C351" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s" s="1">
+        <v>352</v>
+      </c>
+      <c r="C352" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s" s="1">
+        <v>353</v>
+      </c>
+      <c r="C353" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s" s="1">
+        <v>354</v>
+      </c>
+      <c r="C354" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s" s="1">
+        <v>355</v>
+      </c>
+      <c r="C355" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s" s="1">
+        <v>356</v>
+      </c>
+      <c r="C356" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s" s="1">
+        <v>357</v>
+      </c>
+      <c r="C357" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s" s="1">
+        <v>358</v>
+      </c>
+      <c r="C358" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s" s="1">
+        <v>359</v>
+      </c>
+      <c r="C359" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s" s="1">
+        <v>360</v>
+      </c>
+      <c r="C360" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s" s="1">
+        <v>361</v>
+      </c>
+      <c r="C361" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s" s="1">
+        <v>362</v>
+      </c>
+      <c r="C362" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="s" s="1">
+        <v>363</v>
+      </c>
+      <c r="C363" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="s" s="1">
+        <v>364</v>
+      </c>
+      <c r="C364" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="s" s="1">
+        <v>365</v>
+      </c>
+      <c r="C365" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="s" s="1">
+        <v>366</v>
+      </c>
+      <c r="C366" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="s" s="1">
+        <v>367</v>
+      </c>
+      <c r="C367" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="s" s="1">
+        <v>368</v>
+      </c>
+      <c r="C368" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="s" s="1">
+        <v>369</v>
+      </c>
+      <c r="C369" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="s" s="1">
+        <v>370</v>
+      </c>
+      <c r="C370" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="s" s="1">
+        <v>371</v>
+      </c>
+      <c r="C371" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="s" s="1">
+        <v>372</v>
+      </c>
+      <c r="C372" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="s" s="1">
+        <v>373</v>
+      </c>
+      <c r="C373" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="s" s="1">
+        <v>374</v>
+      </c>
+      <c r="C374" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="s" s="1">
+        <v>375</v>
+      </c>
+      <c r="C375" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="s" s="1">
+        <v>376</v>
+      </c>
+      <c r="C376" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s" s="1">
+        <v>377</v>
+      </c>
+      <c r="C377" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s" s="1">
+        <v>378</v>
+      </c>
+      <c r="C378" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="s" s="1">
+        <v>379</v>
+      </c>
+      <c r="C379" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="s" s="1">
+        <v>380</v>
+      </c>
+      <c r="C380" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s" s="1">
+        <v>381</v>
+      </c>
+      <c r="C381" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="s" s="1">
+        <v>382</v>
+      </c>
+      <c r="C382" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="s" s="1">
+        <v>383</v>
+      </c>
+      <c r="C383" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="s" s="1">
+        <v>384</v>
+      </c>
+      <c r="C384" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="s" s="1">
+        <v>385</v>
+      </c>
+      <c r="C385" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="s" s="1">
+        <v>386</v>
+      </c>
+      <c r="C386" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="s" s="1">
+        <v>387</v>
+      </c>
+      <c r="C387" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="s" s="1">
+        <v>388</v>
+      </c>
+      <c r="C388" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="s" s="1">
+        <v>389</v>
+      </c>
+      <c r="C389" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="s" s="1">
+        <v>390</v>
+      </c>
+      <c r="C390" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="s" s="1">
+        <v>391</v>
+      </c>
+      <c r="C391" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="s" s="1">
+        <v>392</v>
+      </c>
+      <c r="C392" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="s" s="1">
+        <v>393</v>
+      </c>
+      <c r="C393" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="s" s="1">
+        <v>394</v>
+      </c>
+      <c r="C394" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="s" s="1">
+        <v>395</v>
+      </c>
+      <c r="C395" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="s" s="1">
+        <v>396</v>
+      </c>
+      <c r="C396" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="s" s="1">
+        <v>397</v>
+      </c>
+      <c r="C397" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="s" s="1">
+        <v>398</v>
+      </c>
+      <c r="C398" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="s" s="1">
+        <v>399</v>
+      </c>
+      <c r="C399" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="s" s="1">
+        <v>400</v>
+      </c>
+      <c r="C400" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="s" s="1">
+        <v>401</v>
+      </c>
+      <c r="C401" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="s" s="1">
+        <v>402</v>
+      </c>
+      <c r="C402" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="s" s="1">
+        <v>403</v>
+      </c>
+      <c r="C403" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="s" s="1">
+        <v>404</v>
+      </c>
+      <c r="C404" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="s" s="1">
+        <v>405</v>
+      </c>
+      <c r="C405" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="s" s="1">
+        <v>406</v>
+      </c>
+      <c r="C406" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="s" s="1">
+        <v>407</v>
+      </c>
+      <c r="C407" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="s" s="1">
+        <v>408</v>
+      </c>
+      <c r="C408" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="s" s="1">
+        <v>409</v>
+      </c>
+      <c r="C409" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="s" s="1">
+        <v>410</v>
+      </c>
+      <c r="C410" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="s" s="1">
+        <v>411</v>
+      </c>
+      <c r="C411" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="s" s="1">
+        <v>412</v>
+      </c>
+      <c r="C412" t="s" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="s" s="1">
+        <v>413</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test updated times 2
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UltimateDignityPlan.xlsx
+++ b/src/test/resources/TestData/UltimateDignityPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48116" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48141" uniqueCount="372">
   <si>
     <t>IDNumber</t>
   </si>
@@ -1055,6 +1055,81 @@
   </si>
   <si>
     <t>8605050059086</t>
+  </si>
+  <si>
+    <t>0805053472082</t>
+  </si>
+  <si>
+    <t>9405051381087</t>
+  </si>
+  <si>
+    <t>9105050484185</t>
+  </si>
+  <si>
+    <t>0805051084186</t>
+  </si>
+  <si>
+    <t>9405054015187</t>
+  </si>
+  <si>
+    <t>96050533240810</t>
+  </si>
+  <si>
+    <t>9605052815088</t>
+  </si>
+  <si>
+    <t>9605051240189</t>
+  </si>
+  <si>
+    <t>9605050620183</t>
+  </si>
+  <si>
+    <t>96050516500810</t>
+  </si>
+  <si>
+    <t>86050540360810</t>
+  </si>
+  <si>
+    <t>8605051812087</t>
+  </si>
+  <si>
+    <t>86050505900810</t>
+  </si>
+  <si>
+    <t>8605052718085</t>
+  </si>
+  <si>
+    <t>8605051876082</t>
+  </si>
+  <si>
+    <t>9605052337182</t>
+  </si>
+  <si>
+    <t>9605054854085</t>
+  </si>
+  <si>
+    <t>91050525460810</t>
+  </si>
+  <si>
+    <t>9105050846185</t>
+  </si>
+  <si>
+    <t>8805052747189</t>
+  </si>
+  <si>
+    <t>8805050407083</t>
+  </si>
+  <si>
+    <t>8805052090184</t>
+  </si>
+  <si>
+    <t>8805050646086</t>
+  </si>
+  <si>
+    <t>8805053064089</t>
+  </si>
+  <si>
+    <t>8805054951185</t>
   </si>
 </sst>
 </file>
@@ -1405,7 +1480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C349"/>
+  <dimension ref="A1:C374"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
@@ -4141,6 +4216,131 @@
         <v>346</v>
       </c>
     </row>
+    <row r="350">
+      <c r="A350" t="s" s="1">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s" s="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s" s="1">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s" s="1">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s" s="1">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s" s="1">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s" s="1">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s" s="1">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s" s="1">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s" s="1">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s" s="1">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s" s="1">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="s" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="s" s="1">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="s" s="1">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="s" s="1">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="s" s="1">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="s" s="1">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="s" s="1">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="s" s="1">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="s" s="1">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="s" s="1">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="s" s="1">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="s" s="1">
+        <v>371</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added New Java Class into 1 Page
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/UltimateDignityPlan.xlsx
+++ b/src/test/resources/TestData/UltimateDignityPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48141" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48145" uniqueCount="376">
   <si>
     <t>IDNumber</t>
   </si>
@@ -1130,6 +1130,18 @@
   </si>
   <si>
     <t>8805054951185</t>
+  </si>
+  <si>
+    <t>9705050142186</t>
+  </si>
+  <si>
+    <t>9005052089182</t>
+  </si>
+  <si>
+    <t>9005053564183</t>
+  </si>
+  <si>
+    <t>9005053597084</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C374"/>
+  <dimension ref="A1:C378"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
@@ -4341,6 +4353,26 @@
         <v>371</v>
       </c>
     </row>
+    <row r="375">
+      <c r="A375" t="s" s="1">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="s" s="1">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s" s="1">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s" s="1">
+        <v>375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>